<commit_message>
implemented --catfile flag to provide captions for abbreviated criteria
</commit_message>
<xml_diff>
--- a/examples/example.xlsx
+++ b/examples/example.xlsx
@@ -37,16 +37,16 @@
     <t xml:space="preserve">Note</t>
   </si>
   <si>
-    <t xml:space="preserve">Inhalt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rechtschreibung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kommentar</t>
+    <t xml:space="preserve">cont</t>
+  </si>
+  <si>
+    <t xml:space="preserve">styl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comm</t>
   </si>
   <si>
     <t xml:space="preserve">Points</t>
@@ -210,20 +210,21 @@
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="47.02"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>